<commit_message>
beginning to implement timer and mmu project cleanup
</commit_message>
<xml_diff>
--- a/architektur/MMIO_Regs.xlsx
+++ b/architektur/MMIO_Regs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Entwicklung\SixteenShadesOfCpu\architektur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Entwicklung\SixteenShadesOfCpu\architektur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC4EDAA0-E13B-4B44-B35A-0C378F793969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5467A24C-A8D5-4E98-A17D-81958613FD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10320" yWindow="4035" windowWidth="36195" windowHeight="15435" xr2:uid="{7A8374FD-2670-4672-9ADB-6B88427E43CB}"/>
+    <workbookView xWindow="5520" yWindow="765" windowWidth="21600" windowHeight="12645" xr2:uid="{7A8374FD-2670-4672-9ADB-6B88427E43CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>btn_conig</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>ob das reset signal weitergereicht wird.</t>
+  </si>
+  <si>
+    <t>3 downto 2</t>
   </si>
 </sst>
 </file>
@@ -200,8 +203,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -538,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719CEA00-8279-4313-9409-BE9B19F58C2A}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,8 +582,7 @@
         <v>15</v>
       </c>
       <c r="O1">
-        <f>SUM(O2:O10)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -607,6 +610,9 @@
       <c r="K2">
         <v>16</v>
       </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
       <c r="N2" t="s">
         <v>19</v>
       </c>
@@ -645,6 +651,9 @@
       <c r="L3" t="s">
         <v>38</v>
       </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
       <c r="N3" t="s">
         <v>20</v>
       </c>
@@ -683,6 +692,9 @@
       <c r="L4" t="s">
         <v>37</v>
       </c>
+      <c r="M4" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="N4" t="s">
         <v>21</v>
       </c>
@@ -706,6 +718,9 @@
       <c r="L5" t="s">
         <v>36</v>
       </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
       <c r="N5" t="s">
         <v>22</v>
       </c>
@@ -723,6 +738,9 @@
       <c r="L6" t="s">
         <v>35</v>
       </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
       <c r="N6" t="s">
         <v>23</v>
       </c>
@@ -734,6 +752,9 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>6</v>
+      </c>
       <c r="N7" t="s">
         <v>24</v>
       </c>
@@ -745,6 +766,9 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>7</v>
+      </c>
       <c r="N8" t="s">
         <v>25</v>
       </c>
@@ -756,6 +780,9 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>8</v>
+      </c>
       <c r="N9" t="s">
         <v>26</v>
       </c>
@@ -767,6 +794,9 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>9</v>
+      </c>
       <c r="N10" t="s">
         <v>27</v>
       </c>
@@ -778,6 +808,9 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>10</v>
+      </c>
       <c r="N11" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
added timer0 to mmio and removed not needed pins from cc and mmu
</commit_message>
<xml_diff>
--- a/architektur/MMIO_Regs.xlsx
+++ b/architektur/MMIO_Regs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Entwicklung\SixteenShadesOfCpu\architektur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Entwicklung\SixteenShadesOfCpu\architektur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5467A24C-A8D5-4E98-A17D-81958613FD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE525E8-DB8C-4DD6-8C45-815E699E000D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="765" windowWidth="21600" windowHeight="12645" xr2:uid="{7A8374FD-2670-4672-9ADB-6B88427E43CB}"/>
+    <workbookView xWindow="7395" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{7A8374FD-2670-4672-9ADB-6B88427E43CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
-    <t>btn_conig</t>
-  </si>
-  <si>
     <t>size</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>3 downto 2</t>
+  </si>
+  <si>
+    <t>btn_config</t>
   </si>
 </sst>
 </file>
@@ -203,9 +203,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -543,7 +542,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,31 +554,31 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
         <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
       </c>
       <c r="O1">
         <v>11</v>
@@ -587,25 +586,25 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2">
         <v>16</v>
@@ -614,89 +613,89 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3">
         <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4">
         <v>16</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O4">
         <v>2</v>
@@ -704,51 +703,51 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5">
         <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
         <v>34</v>
-      </c>
-      <c r="L6" t="s">
-        <v>35</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -756,13 +755,13 @@
         <v>6</v>
       </c>
       <c r="N7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O7">
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -770,13 +769,13 @@
         <v>7</v>
       </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O8">
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -784,13 +783,13 @@
         <v>8</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -798,13 +797,13 @@
         <v>9</v>
       </c>
       <c r="N10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -812,13 +811,13 @@
         <v>10</v>
       </c>
       <c r="N11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>